<commit_message>
Most of Quartiles and Plots
</commit_message>
<xml_diff>
--- a/data/Study_results.xlsx
+++ b/data/Study_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d949fffeeafd9ab/Documents/GitHub/-pymaceuticals-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F71946F-98A7-4CAA-B834-B8924AC95969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3F71946F-98A7-4CAA-B834-B8924AC95969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF284E5-2F86-4F3F-9ECB-45CE49EE8741}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B32CACB-EE47-4ED6-98E6-C5491C1580C4}"/>
   </bookViews>
@@ -1641,9 +1641,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC0B065-E5A7-47A2-AE0B-212F1945F1CC}">
   <dimension ref="A1:D1894"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>